<commit_message>
- added more test cases and handled them
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/TryToLoad/PrintareaInvalidFormula.xlsx
+++ b/ClosedXML_Tests/Resource/TryToLoad/PrintareaInvalidFormula.xlsx
@@ -1,20 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51ED3BF-DEE2-4532-88CA-D9941C043F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5E4BF3-7CD2-4FE6-BB37-FF931E4D4B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1!" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'[1]Tabelle2!'!$A$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">UNGÜLTIG</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -122,19 +119,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Tabelle2!"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,7 +387,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>